<commit_message>
Improved CAOSCE_RESULT script to include PAPER I and II
</commit_message>
<xml_diff>
--- a/EXAMS_INTERNAL/CAOSCE_RESULT/RAW_CAOSCE_RESULT/VIVA.xlsx
+++ b/EXAMS_INTERNAL/CAOSCE_RESULT/RAW_CAOSCE_RESULT/VIVA.xlsx
@@ -60,7 +60,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E3"/>
   <sheetData>
     <row r="1" spans="1:5" customHeight="0">
       <c r="A1" s="0" t="inlineStr">
@@ -92,17 +92,17 @@
     <row r="2" spans="1:5" customHeight="0">
       <c r="A2" s="0" t="inlineStr">
         <is>
-          <t>OMEDE OJOMA VIRTUOUS BN/A23/002</t>
+          <t>UDEM CHINECHEREM CHISOM BN/A23/010</t>
         </is>
       </c>
       <c r="C2" s="0" t="inlineStr">
         <is>
-          <t>yanuueyey@gmail.com1</t>
+          <t>yanuueyey@gmail.com9</t>
         </is>
       </c>
       <c r="D2" s="0" t="inlineStr">
         <is>
-          <t>Monday, 24 November 2025, 9:25 PM</t>
+          <t>Sunday, 30 November 2025, 4:52 PM</t>
         </is>
       </c>
       <c r="E2" s="0" t="inlineStr">
@@ -114,88 +114,22 @@
     <row r="3" spans="1:5" customHeight="0">
       <c r="A3" s="0" t="inlineStr">
         <is>
-          <t>NDIFE LUCY IFEOMA BN/A23/003</t>
+          <t>IKEJIAKU LILIAN CHIAMAKA BN/A23/011</t>
         </is>
       </c>
       <c r="C3" s="0" t="inlineStr">
         <is>
-          <t>yanuueyey@gmail.com2</t>
+          <t>yanuueyey@gmail.com10</t>
         </is>
       </c>
       <c r="D3" s="0" t="inlineStr">
         <is>
-          <t>Monday, 24 November 2025, 5:27 PM</t>
+          <t>Sunday, 30 November 2025, 4:58 PM</t>
         </is>
       </c>
       <c r="E3" s="0" t="inlineStr">
         <is>
-          <t>5</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" spans="1:5" customHeight="0">
-      <c r="A4" s="0" t="inlineStr">
-        <is>
-          <t>EGWUONWU EBUBECHI COMFORT BN/A23/004</t>
-        </is>
-      </c>
-      <c r="C4" s="0" t="inlineStr">
-        <is>
-          <t>yanuueyey@gmail.com3</t>
-        </is>
-      </c>
-      <c r="D4" s="0" t="inlineStr">
-        <is>
-          <t>Monday, 24 November 2025, 5:24 PM</t>
-        </is>
-      </c>
-      <c r="E4" s="0" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" spans="1:5" customHeight="0">
-      <c r="A5" s="0" t="inlineStr">
-        <is>
-          <t>MUHAMMAD KHADIJA ABDULLAHI BN/A23/005</t>
-        </is>
-      </c>
-      <c r="C5" s="0" t="inlineStr">
-        <is>
-          <t>yanuueyey@gmail.com4</t>
-        </is>
-      </c>
-      <c r="D5" s="0" t="inlineStr">
-        <is>
-          <t>Monday, 24 November 2025, 5:16 PM</t>
-        </is>
-      </c>
-      <c r="E5" s="0" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
-      </c>
-    </row>
-    <row r="6" spans="1:5" customHeight="0">
-      <c r="A6" s="0" t="inlineStr">
-        <is>
-          <t>UMORU AHUOIZA JEMIMA BN/A23/006</t>
-        </is>
-      </c>
-      <c r="C6" s="0" t="inlineStr">
-        <is>
-          <t>yanuueyey@gmail.com5</t>
-        </is>
-      </c>
-      <c r="D6" s="0" t="inlineStr">
-        <is>
-          <t>Monday, 24 November 2025, 5:21 PM</t>
-        </is>
-      </c>
-      <c r="E6" s="0" t="inlineStr">
-        <is>
-          <t>6.5</t>
+          <t>10</t>
         </is>
       </c>
     </row>

</xml_diff>